<commit_message>
Better bom, new eagle.py script
</commit_message>
<xml_diff>
--- a/cc_power_supply/rev_a/cc_power_supply_bom.xlsx
+++ b/cc_power_supply/rev_a/cc_power_supply_bom.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="68">
   <si>
     <t>Qty</t>
   </si>
@@ -38,6 +38,12 @@
     <t>DIGIKEY</t>
   </si>
   <si>
+    <t>DIGIREEL</t>
+  </si>
+  <si>
+    <t>MOUSER</t>
+  </si>
+  <si>
     <t>0.1uF</t>
   </si>
   <si>
@@ -56,6 +62,9 @@
     <t>445-1316-1-ND</t>
   </si>
   <si>
+    <t>445-1316-6-ND</t>
+  </si>
+  <si>
     <t>1uF</t>
   </si>
   <si>
@@ -65,6 +74,9 @@
     <t>445-1321-1-ND</t>
   </si>
   <si>
+    <t>445-1321-6-ND</t>
+  </si>
+  <si>
     <t>4.7uF</t>
   </si>
   <si>
@@ -74,6 +86,9 @@
     <t>445-5178-1-ND</t>
   </si>
   <si>
+    <t>445-5178-6-ND</t>
+  </si>
+  <si>
     <t>10uF</t>
   </si>
   <si>
@@ -89,6 +104,9 @@
     <t>399-8152-1-ND</t>
   </si>
   <si>
+    <t>399-8152-6-ND</t>
+  </si>
+  <si>
     <t>47uF</t>
   </si>
   <si>
@@ -107,6 +125,9 @@
     <t>399-3700-1-ND</t>
   </si>
   <si>
+    <t>399-3700-6-ND</t>
+  </si>
+  <si>
     <t>100uF 25V</t>
   </si>
   <si>
@@ -119,6 +140,12 @@
     <t>399-5175-1-ND</t>
   </si>
   <si>
+    <t>399-5175-6-ND</t>
+  </si>
+  <si>
+    <t>DNP</t>
+  </si>
+  <si>
     <t>SCREW-TERMINAL_2_0.100</t>
   </si>
   <si>
@@ -149,6 +176,9 @@
     <t>587-1625-1-ND</t>
   </si>
   <si>
+    <t>587-1625-6-ND</t>
+  </si>
+  <si>
     <t>NCHAN_MOSFET</t>
   </si>
   <si>
@@ -156,6 +186,12 @@
   </si>
   <si>
     <t>SI1302DL-T1-GE3CT-ND</t>
+  </si>
+  <si>
+    <t>SI1302DL-T1-GE3DKR-ND</t>
+  </si>
+  <si>
+    <t>781-SI1302DL-E3</t>
   </si>
   <si>
     <t>LTC3588_</t>
@@ -305,22 +341,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E3" activeCellId="0" pane="topLeft" sqref="E3"/>
+      <selection activeCell="D13" activeCellId="0" pane="topLeft" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.47959183673469"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="25.3265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="30.1938775510204"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.7448979591837"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.9948979591837"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.9183673469388"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.2448979591837"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.1020408163265"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.7397959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
@@ -345,28 +382,37 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
@@ -374,22 +420,25 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>11</v>
-      </c>
       <c r="G3" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
@@ -397,22 +446,25 @@
         <v>1</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>18</v>
+        <v>22</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
@@ -420,22 +472,25 @@
         <v>1</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>23</v>
+        <v>28</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
@@ -443,22 +498,25 @@
         <v>1</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>29</v>
+        <v>35</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
@@ -466,42 +524,45 @@
         <v>5</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>33</v>
+        <v>40</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
-      <c r="A8" s="0" t="n">
-        <v>1</v>
+      <c r="A8" s="0" t="s">
+        <v>42</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
@@ -509,22 +570,25 @@
         <v>1</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D9" s="2" t="n">
         <v>1210</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>43</v>
+        <v>52</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>53</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
@@ -532,19 +596,25 @@
         <v>2</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>46</v>
+        <v>56</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>58</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
@@ -552,51 +622,53 @@
         <v>1</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>51</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="I11" s="3"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
-      <c r="A12" s="0" t="n">
-        <v>1</v>
+      <c r="A12" s="0" t="s">
+        <v>42</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="I12" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05416666666667" bottom="0.7875" header="0.7875" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="landscape" pageOrder="downThenOver" paperSize="1" scale="57" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="landscape" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;F</oddHeader>
     <oddFooter/>

</xml_diff>